<commit_message>
Style input type file button, change projects template
</commit_message>
<xml_diff>
--- a/public/templates/en_template.xlsx
+++ b/public/templates/en_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Topics" sheetId="1" state="visible" r:id="rId2"/>
@@ -119,7 +119,7 @@
     <t xml:space="preserve">Master</t>
   </si>
   <si>
-    <t xml:space="preserve">Technologica Work</t>
+    <t xml:space="preserve">Technological Work</t>
   </si>
   <si>
     <t xml:space="preserve">Katedra projektowania Architektoniczno-Budowlanego</t>
@@ -370,11 +370,11 @@
   </sheetPr>
   <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="38.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.57"/>
@@ -1598,11 +1598,11 @@
   </sheetPr>
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.81"/>

</xml_diff>